<commit_message>
arrange connectors' pins by pinID
</commit_message>
<xml_diff>
--- a/IO map.xlsx
+++ b/IO map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="11280" windowHeight="4950"/>
@@ -12,12 +12,11 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="129">
   <si>
     <t>DI</t>
   </si>
@@ -409,8 +408,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -462,9 +461,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,9 +482,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office тема">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -520,9 +522,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,10 +556,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,10 +590,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -765,14 +765,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -780,9 +780,10 @@
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -822,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -842,7 +843,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -862,7 +863,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -876,7 +877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -890,7 +891,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -904,7 +905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
@@ -918,7 +919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
@@ -932,7 +933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
@@ -940,7 +941,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -948,23 +949,33 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:23">
+      <c r="A13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="G13" s="4" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="G13" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="M13" s="4" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="M13" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="5"/>
+      <c r="Q13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="U13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="3" t="s">
         <v>128</v>
       </c>
@@ -985,8 +996,26 @@
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>78</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -1011,8 +1040,26 @@
       <c r="N15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>90</v>
+      </c>
+      <c r="R15" t="s">
+        <v>57</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>126</v>
+      </c>
+      <c r="V15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -1037,8 +1084,26 @@
       <c r="N16" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>91</v>
+      </c>
+      <c r="R16" t="s">
+        <v>58</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="U16" t="s">
+        <v>125</v>
+      </c>
+      <c r="V16" t="s">
+        <v>59</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1057,8 +1122,26 @@
       <c r="I17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>93</v>
+      </c>
+      <c r="R17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="U17" t="s">
+        <v>109</v>
+      </c>
+      <c r="V17" t="s">
+        <v>41</v>
+      </c>
+      <c r="W17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -1077,8 +1160,26 @@
       <c r="I18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>103</v>
+      </c>
+      <c r="R18" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18">
+        <v>4</v>
+      </c>
+      <c r="U18" t="s">
+        <v>117</v>
+      </c>
+      <c r="V18" t="s">
+        <v>49</v>
+      </c>
+      <c r="W18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -1097,8 +1198,26 @@
       <c r="I19">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>94</v>
+      </c>
+      <c r="R19" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19">
+        <v>5</v>
+      </c>
+      <c r="U19" t="s">
+        <v>110</v>
+      </c>
+      <c r="V19" t="s">
+        <v>42</v>
+      </c>
+      <c r="W19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -1117,8 +1236,26 @@
       <c r="I20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>104</v>
+      </c>
+      <c r="R20" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20">
+        <v>6</v>
+      </c>
+      <c r="U20" t="s">
+        <v>118</v>
+      </c>
+      <c r="V20" t="s">
+        <v>50</v>
+      </c>
+      <c r="W20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -1137,8 +1274,26 @@
       <c r="I21">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>95</v>
+      </c>
+      <c r="R21" t="s">
+        <v>27</v>
+      </c>
+      <c r="S21">
+        <v>7</v>
+      </c>
+      <c r="U21" t="s">
+        <v>111</v>
+      </c>
+      <c r="V21" t="s">
+        <v>43</v>
+      </c>
+      <c r="W21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -1157,8 +1312,26 @@
       <c r="I22">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>105</v>
+      </c>
+      <c r="R22" t="s">
+        <v>35</v>
+      </c>
+      <c r="S22">
+        <v>8</v>
+      </c>
+      <c r="U22" t="s">
+        <v>119</v>
+      </c>
+      <c r="V22" t="s">
+        <v>51</v>
+      </c>
+      <c r="W22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -1177,8 +1350,26 @@
       <c r="I23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>96</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23">
+        <v>9</v>
+      </c>
+      <c r="U23" t="s">
+        <v>112</v>
+      </c>
+      <c r="V23" t="s">
+        <v>44</v>
+      </c>
+      <c r="W23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -1197,8 +1388,26 @@
       <c r="I24">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>106</v>
+      </c>
+      <c r="R24" t="s">
+        <v>36</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="U24" t="s">
+        <v>120</v>
+      </c>
+      <c r="V24" t="s">
+        <v>52</v>
+      </c>
+      <c r="W24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -1217,8 +1426,26 @@
       <c r="I25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>97</v>
+      </c>
+      <c r="R25" t="s">
+        <v>29</v>
+      </c>
+      <c r="S25">
+        <v>11</v>
+      </c>
+      <c r="U25" t="s">
+        <v>113</v>
+      </c>
+      <c r="V25" t="s">
+        <v>45</v>
+      </c>
+      <c r="W25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -1237,8 +1464,26 @@
       <c r="I26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>107</v>
+      </c>
+      <c r="R26" t="s">
+        <v>37</v>
+      </c>
+      <c r="S26">
+        <v>12</v>
+      </c>
+      <c r="U26" t="s">
+        <v>121</v>
+      </c>
+      <c r="V26" t="s">
+        <v>53</v>
+      </c>
+      <c r="W26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -1257,8 +1502,26 @@
       <c r="I27">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>98</v>
+      </c>
+      <c r="R27" t="s">
+        <v>30</v>
+      </c>
+      <c r="S27">
+        <v>13</v>
+      </c>
+      <c r="U27" t="s">
+        <v>115</v>
+      </c>
+      <c r="V27" t="s">
+        <v>46</v>
+      </c>
+      <c r="W27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>101</v>
       </c>
@@ -1277,8 +1540,26 @@
       <c r="I28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>101</v>
+      </c>
+      <c r="R28" t="s">
+        <v>38</v>
+      </c>
+      <c r="S28">
+        <v>14</v>
+      </c>
+      <c r="U28" t="s">
+        <v>122</v>
+      </c>
+      <c r="V28" t="s">
+        <v>54</v>
+      </c>
+      <c r="W28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -1297,8 +1578,26 @@
       <c r="I29">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>99</v>
+      </c>
+      <c r="R29" t="s">
+        <v>31</v>
+      </c>
+      <c r="S29">
+        <v>15</v>
+      </c>
+      <c r="U29" t="s">
+        <v>114</v>
+      </c>
+      <c r="V29" t="s">
+        <v>47</v>
+      </c>
+      <c r="W29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -1317,8 +1616,26 @@
       <c r="I30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>100</v>
+      </c>
+      <c r="R30" t="s">
+        <v>39</v>
+      </c>
+      <c r="S30">
+        <v>16</v>
+      </c>
+      <c r="U30" t="s">
+        <v>123</v>
+      </c>
+      <c r="V30" t="s">
+        <v>55</v>
+      </c>
+      <c r="W30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1337,8 +1654,26 @@
       <c r="I31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>102</v>
+      </c>
+      <c r="R31" t="s">
+        <v>32</v>
+      </c>
+      <c r="S31">
+        <v>17</v>
+      </c>
+      <c r="U31" t="s">
+        <v>116</v>
+      </c>
+      <c r="V31" t="s">
+        <v>48</v>
+      </c>
+      <c r="W31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -1357,8 +1692,26 @@
       <c r="I32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>108</v>
+      </c>
+      <c r="R32" t="s">
+        <v>40</v>
+      </c>
+      <c r="S32">
+        <v>18</v>
+      </c>
+      <c r="U32" t="s">
+        <v>124</v>
+      </c>
+      <c r="V32" t="s">
+        <v>56</v>
+      </c>
+      <c r="W32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -1377,12 +1730,35 @@
       <c r="I33">
         <v>19</v>
       </c>
+      <c r="Q33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R33" t="s">
+        <v>88</v>
+      </c>
+      <c r="S33">
+        <v>19</v>
+      </c>
+      <c r="U33" t="s">
+        <v>127</v>
+      </c>
+      <c r="V33" t="s">
+        <v>89</v>
+      </c>
+      <c r="W33">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <sortState ref="U15:W33">
+    <sortCondition ref="W15:W33"/>
+  </sortState>
+  <mergeCells count="5">
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="G13:I13"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="U13:W13"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1390,12 +1766,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1403,12 +1779,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>